<commit_message>
work in progress 2
</commit_message>
<xml_diff>
--- a/Worked_datasets/dataset_tableau.xlsx
+++ b/Worked_datasets/dataset_tableau.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:R126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>sol_min</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Receita_ha</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Receita_ajustada</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -534,7 +544,7 @@
         <v>9814.28618655</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -553,9 +563,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
         <v>6</v>
@@ -565,6 +573,12 @@
       </c>
       <c r="P2" t="n">
         <v>8</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1583.49667640544</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1187.62250730408</v>
       </c>
     </row>
     <row r="3">
@@ -601,11 +615,9 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>6</v>
@@ -616,6 +628,12 @@
       <c r="P3" t="n">
         <v>10</v>
       </c>
+      <c r="Q3" t="n">
+        <v>2921.7091938</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2921.7091938</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -654,13 +672,9 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="K4" t="n">
-        <v>2</v>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>2</v>
-      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
         <v>6.5</v>
       </c>
@@ -668,6 +682,12 @@
         <v>7.5</v>
       </c>
       <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="n">
+        <v>1860.789316201096</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1240.52621080073</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -705,12 +725,8 @@
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>2</v>
-      </c>
-      <c r="M5" t="n">
-        <v>2</v>
-      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
         <v>6</v>
       </c>
@@ -720,6 +736,12 @@
       <c r="P5" t="n">
         <v>6</v>
       </c>
+      <c r="Q5" t="n">
+        <v>3779.058857384692</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3779.058857384692</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -756,9 +778,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>2</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
@@ -770,6 +790,12 @@
       <c r="P6" t="n">
         <v>10</v>
       </c>
+      <c r="Q6" t="n">
+        <v>2806.478067272727</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2806.478067272727</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -808,12 +834,8 @@
       <c r="J7" t="n">
         <v>3</v>
       </c>
-      <c r="K7" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>6</v>
@@ -824,6 +846,12 @@
       <c r="P7" t="n">
         <v>6</v>
       </c>
+      <c r="Q7" t="n">
+        <v>5114.726619009901</v>
+      </c>
+      <c r="R7" t="n">
+        <v>5114.726619009901</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -862,9 +890,7 @@
       <c r="J8" t="n">
         <v>3</v>
       </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
@@ -876,6 +902,12 @@
       <c r="P8" t="n">
         <v>6</v>
       </c>
+      <c r="Q8" t="n">
+        <v>2789.310949906872</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2789.310949906872</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -912,12 +944,8 @@
         <v>2</v>
       </c>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L9" t="n">
-        <v>2</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
         <v>6</v>
@@ -928,6 +956,12 @@
       <c r="P9" t="n">
         <v>10</v>
       </c>
+      <c r="Q9" t="n">
+        <v>3427.92</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3427.92</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -966,15 +1000,9 @@
       <c r="J10" t="n">
         <v>3</v>
       </c>
-      <c r="K10" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" t="n">
-        <v>2</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>6</v>
       </c>
@@ -984,6 +1012,12 @@
       <c r="P10" t="n">
         <v>6</v>
       </c>
+      <c r="Q10" t="n">
+        <v>2351.569232194212</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2351.569232194212</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1020,13 +1054,9 @@
         <v>1</v>
       </c>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>2</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
-        <v>2</v>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
         <v>5.5</v>
       </c>
@@ -1036,6 +1066,12 @@
       <c r="P11" t="n">
         <v>6</v>
       </c>
+      <c r="Q11" t="n">
+        <v>1814.570221396475</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1814.570221396475</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1077,9 +1113,7 @@
       <c r="K12" t="n">
         <v>2</v>
       </c>
-      <c r="L12" t="n">
-        <v>2</v>
-      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
         <v>5.5</v>
@@ -1090,6 +1124,12 @@
       <c r="P12" t="n">
         <v>6</v>
       </c>
+      <c r="Q12" t="n">
+        <v>1678.412719357611</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1678.412719357611</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1131,12 +1171,8 @@
       <c r="K13" t="n">
         <v>2</v>
       </c>
-      <c r="L13" t="n">
-        <v>2</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2</v>
-      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>5.5</v>
       </c>
@@ -1146,6 +1182,12 @@
       <c r="P13" t="n">
         <v>8</v>
       </c>
+      <c r="Q13" t="n">
+        <v>1932.547309473375</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1932.547309473375</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1184,13 +1226,11 @@
       <c r="J14" t="n">
         <v>3</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="n">
-        <v>2</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2</v>
-      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
         <v>5.5</v>
       </c>
@@ -1200,6 +1240,12 @@
       <c r="P14" t="n">
         <v>8</v>
       </c>
+      <c r="Q14" t="n">
+        <v>1171.211222853634</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1171.211222853634</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1220,7 +1266,7 @@
         <v>22731.825175542</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1239,11 +1285,9 @@
         <v>3</v>
       </c>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="n">
-        <v>2</v>
-      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15" t="n">
         <v>5.5</v>
@@ -1254,6 +1298,12 @@
       <c r="P15" t="n">
         <v>8</v>
       </c>
+      <c r="Q15" t="n">
+        <v>680.5750665662555</v>
+      </c>
+      <c r="R15" t="n">
+        <v>510.4312999246916</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1295,12 +1345,8 @@
       <c r="K16" t="n">
         <v>2</v>
       </c>
-      <c r="L16" t="n">
-        <v>2</v>
-      </c>
-      <c r="M16" t="n">
-        <v>2</v>
-      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>5.5</v>
       </c>
@@ -1310,6 +1356,12 @@
       <c r="P16" t="n">
         <v>6</v>
       </c>
+      <c r="Q16" t="n">
+        <v>1534.409676521068</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1534.409676521068</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1351,9 +1403,7 @@
       <c r="K17" t="n">
         <v>2</v>
       </c>
-      <c r="L17" t="n">
-        <v>2</v>
-      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>5.5</v>
@@ -1364,6 +1414,12 @@
       <c r="P17" t="n">
         <v>6</v>
       </c>
+      <c r="Q17" t="n">
+        <v>2537.421680567933</v>
+      </c>
+      <c r="R17" t="n">
+        <v>2537.421680567933</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1401,14 +1457,10 @@
         <v>3</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" t="n">
-        <v>2</v>
-      </c>
-      <c r="M18" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
         <v>6</v>
       </c>
@@ -1418,6 +1470,12 @@
       <c r="P18" t="n">
         <v>8</v>
       </c>
+      <c r="Q18" t="n">
+        <v>8218.931689819005</v>
+      </c>
+      <c r="R18" t="n">
+        <v>6164.198767364253</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1455,12 +1513,10 @@
         <v>3</v>
       </c>
       <c r="K19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
-        <v>2</v>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
         <v>6</v>
       </c>
@@ -1469,6 +1525,12 @@
       </c>
       <c r="P19" t="n">
         <v>8</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>8218.931689819005</v>
+      </c>
+      <c r="R19" t="n">
+        <v>6164.198767364253</v>
       </c>
     </row>
     <row r="20">
@@ -1518,6 +1580,12 @@
       <c r="P20" t="n">
         <v>12</v>
       </c>
+      <c r="Q20" t="n">
+        <v>1818.019786285698</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1818.019786285698</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1557,14 +1625,10 @@
         <v>3</v>
       </c>
       <c r="K21" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" t="n">
-        <v>2</v>
-      </c>
-      <c r="M21" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>5.5</v>
       </c>
@@ -1574,6 +1638,12 @@
       <c r="P21" t="n">
         <v>6</v>
       </c>
+      <c r="Q21" t="n">
+        <v>1950.8941178031</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1463.170588352325</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1592,7 +1662,7 @@
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1611,9 +1681,7 @@
         <v>3</v>
       </c>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="n">
-        <v>1</v>
-      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>6</v>
@@ -1624,6 +1692,8 @@
       <c r="P22" t="n">
         <v>8</v>
       </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1659,11 +1729,9 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L23" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
         <v>6</v>
@@ -1674,6 +1742,12 @@
       <c r="P23" t="n">
         <v>10</v>
       </c>
+      <c r="Q23" t="n">
+        <v>3127.956811824</v>
+      </c>
+      <c r="R23" t="n">
+        <v>3127.956811824</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1712,13 +1786,9 @@
       <c r="J24" t="n">
         <v>1</v>
       </c>
-      <c r="K24" t="n">
-        <v>2</v>
-      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
-        <v>2</v>
-      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
         <v>6.5</v>
       </c>
@@ -1726,6 +1796,12 @@
         <v>7.5</v>
       </c>
       <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="n">
+        <v>1707.649287212535</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1138.43285814169</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1763,12 +1839,8 @@
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
-        <v>2</v>
-      </c>
-      <c r="M25" t="n">
-        <v>2</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
         <v>6</v>
       </c>
@@ -1778,6 +1850,12 @@
       <c r="P25" t="n">
         <v>6</v>
       </c>
+      <c r="Q25" t="n">
+        <v>4692.382126594276</v>
+      </c>
+      <c r="R25" t="n">
+        <v>4692.382126594276</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1814,9 +1892,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>2</v>
-      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
@@ -1828,6 +1904,12 @@
       <c r="P26" t="n">
         <v>10</v>
       </c>
+      <c r="Q26" t="n">
+        <v>2059.684612363636</v>
+      </c>
+      <c r="R26" t="n">
+        <v>2059.684612363636</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1866,12 +1948,8 @@
       <c r="J27" t="n">
         <v>3</v>
       </c>
-      <c r="K27" t="n">
-        <v>2</v>
-      </c>
-      <c r="L27" t="n">
-        <v>2</v>
-      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="n">
         <v>6</v>
@@ -1882,6 +1960,12 @@
       <c r="P27" t="n">
         <v>6</v>
       </c>
+      <c r="Q27" t="n">
+        <v>3560.408347861387</v>
+      </c>
+      <c r="R27" t="n">
+        <v>3560.408347861387</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1920,9 +2004,7 @@
       <c r="J28" t="n">
         <v>3</v>
       </c>
-      <c r="K28" t="n">
-        <v>2</v>
-      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
@@ -1934,6 +2016,12 @@
       <c r="P28" t="n">
         <v>6</v>
       </c>
+      <c r="Q28" t="n">
+        <v>3547.312753651603</v>
+      </c>
+      <c r="R28" t="n">
+        <v>3547.312753651603</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1970,12 +2058,8 @@
         <v>2</v>
       </c>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="n">
-        <v>2</v>
-      </c>
-      <c r="L29" t="n">
-        <v>2</v>
-      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="n">
         <v>6</v>
@@ -1986,6 +2070,12 @@
       <c r="P29" t="n">
         <v>10</v>
       </c>
+      <c r="Q29" t="n">
+        <v>3178.485</v>
+      </c>
+      <c r="R29" t="n">
+        <v>3178.485</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2024,15 +2114,9 @@
       <c r="J30" t="n">
         <v>3</v>
       </c>
-      <c r="K30" t="n">
-        <v>2</v>
-      </c>
-      <c r="L30" t="n">
-        <v>2</v>
-      </c>
-      <c r="M30" t="n">
-        <v>2</v>
-      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
       <c r="N30" t="n">
         <v>6</v>
       </c>
@@ -2041,6 +2125,12 @@
       </c>
       <c r="P30" t="n">
         <v>6</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>2451.059473140688</v>
+      </c>
+      <c r="R30" t="n">
+        <v>2451.059473140688</v>
       </c>
     </row>
     <row r="31">
@@ -2076,13 +2166,9 @@
         <v>1</v>
       </c>
       <c r="J31" t="inlineStr"/>
-      <c r="K31" t="n">
-        <v>2</v>
-      </c>
+      <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="n">
-        <v>2</v>
-      </c>
+      <c r="M31" t="inlineStr"/>
       <c r="N31" t="n">
         <v>5.5</v>
       </c>
@@ -2092,6 +2178,8 @@
       <c r="P31" t="n">
         <v>6</v>
       </c>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2133,9 +2221,7 @@
       <c r="K32" t="n">
         <v>2</v>
       </c>
-      <c r="L32" t="n">
-        <v>2</v>
-      </c>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
         <v>5.5</v>
@@ -2146,6 +2232,12 @@
       <c r="P32" t="n">
         <v>6</v>
       </c>
+      <c r="Q32" t="n">
+        <v>2339.100952380952</v>
+      </c>
+      <c r="R32" t="n">
+        <v>2339.100952380952</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2187,9 +2279,7 @@
       <c r="K33" t="n">
         <v>2</v>
       </c>
-      <c r="L33" t="n">
-        <v>2</v>
-      </c>
+      <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
         <v>5.5</v>
@@ -2200,6 +2290,12 @@
       <c r="P33" t="n">
         <v>6</v>
       </c>
+      <c r="Q33" t="n">
+        <v>2766.209319073001</v>
+      </c>
+      <c r="R33" t="n">
+        <v>2766.209319073001</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2241,12 +2337,8 @@
       <c r="K34" t="n">
         <v>2</v>
       </c>
-      <c r="L34" t="n">
-        <v>2</v>
-      </c>
-      <c r="M34" t="n">
-        <v>2</v>
-      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
         <v>5.5</v>
       </c>
@@ -2256,6 +2348,12 @@
       <c r="P34" t="n">
         <v>8</v>
       </c>
+      <c r="Q34" t="n">
+        <v>1917.591846561389</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1917.591846561389</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2294,13 +2392,11 @@
       <c r="J35" t="n">
         <v>3</v>
       </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="n">
-        <v>2</v>
-      </c>
-      <c r="M35" t="n">
-        <v>2</v>
-      </c>
+      <c r="K35" t="n">
+        <v>3</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
       <c r="N35" t="n">
         <v>5.5</v>
       </c>
@@ -2310,6 +2406,12 @@
       <c r="P35" t="n">
         <v>8</v>
       </c>
+      <c r="Q35" t="n">
+        <v>1124.679943086207</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1124.679943086207</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2330,7 +2432,7 @@
         <v>22283.55358308032</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2349,11 +2451,9 @@
         <v>3</v>
       </c>
       <c r="K36" t="inlineStr"/>
-      <c r="L36" t="n">
-        <v>2</v>
-      </c>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N36" t="n">
         <v>5.5</v>
@@ -2364,6 +2464,12 @@
       <c r="P36" t="n">
         <v>8</v>
       </c>
+      <c r="Q36" t="n">
+        <v>693.6563979896248</v>
+      </c>
+      <c r="R36" t="n">
+        <v>520.2422984922187</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2405,12 +2511,8 @@
       <c r="K37" t="n">
         <v>2</v>
       </c>
-      <c r="L37" t="n">
-        <v>2</v>
-      </c>
-      <c r="M37" t="n">
-        <v>2</v>
-      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
       <c r="N37" t="n">
         <v>5.5</v>
       </c>
@@ -2420,6 +2522,12 @@
       <c r="P37" t="n">
         <v>6</v>
       </c>
+      <c r="Q37" t="n">
+        <v>1334.291160290461</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1334.291160290461</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2461,9 +2569,7 @@
       <c r="K38" t="n">
         <v>2</v>
       </c>
-      <c r="L38" t="n">
-        <v>2</v>
-      </c>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="n">
         <v>5.5</v>
@@ -2474,6 +2580,12 @@
       <c r="P38" t="n">
         <v>6</v>
       </c>
+      <c r="Q38" t="n">
+        <v>2248.663772677995</v>
+      </c>
+      <c r="R38" t="n">
+        <v>2248.663772677995</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2511,14 +2623,10 @@
         <v>3</v>
       </c>
       <c r="K39" t="n">
-        <v>1</v>
-      </c>
-      <c r="L39" t="n">
-        <v>2</v>
-      </c>
-      <c r="M39" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
         <v>6</v>
       </c>
@@ -2528,6 +2636,12 @@
       <c r="P39" t="n">
         <v>8</v>
       </c>
+      <c r="Q39" t="n">
+        <v>8703.82454971591</v>
+      </c>
+      <c r="R39" t="n">
+        <v>6527.868412286933</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2565,12 +2679,10 @@
         <v>3</v>
       </c>
       <c r="K40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40" t="inlineStr"/>
-      <c r="M40" t="n">
-        <v>2</v>
-      </c>
+      <c r="M40" t="inlineStr"/>
       <c r="N40" t="n">
         <v>6</v>
       </c>
@@ -2579,6 +2691,12 @@
       </c>
       <c r="P40" t="n">
         <v>8</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>8703.82454971591</v>
+      </c>
+      <c r="R40" t="n">
+        <v>6527.868412286933</v>
       </c>
     </row>
     <row r="41">
@@ -2628,6 +2746,12 @@
       <c r="P41" t="n">
         <v>12</v>
       </c>
+      <c r="Q41" t="n">
+        <v>2003.75870593145</v>
+      </c>
+      <c r="R41" t="n">
+        <v>2003.75870593145</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2667,14 +2791,10 @@
         <v>3</v>
       </c>
       <c r="K42" t="n">
-        <v>1</v>
-      </c>
-      <c r="L42" t="n">
-        <v>2</v>
-      </c>
-      <c r="M42" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
         <v>5.5</v>
       </c>
@@ -2684,6 +2804,12 @@
       <c r="P42" t="n">
         <v>6</v>
       </c>
+      <c r="Q42" t="n">
+        <v>1338.078166782074</v>
+      </c>
+      <c r="R42" t="n">
+        <v>1003.558625086556</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2704,7 +2830,7 @@
         <v>9203.002974200001</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2723,9 +2849,7 @@
         <v>3</v>
       </c>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="n">
-        <v>1</v>
-      </c>
+      <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
         <v>6</v>
@@ -2735,6 +2859,12 @@
       </c>
       <c r="P43" t="n">
         <v>8</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>1484.868521825516</v>
+      </c>
+      <c r="R43" t="n">
+        <v>1113.651391369137</v>
       </c>
     </row>
     <row r="44">
@@ -2771,11 +2901,9 @@
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="n">
-        <v>2</v>
-      </c>
-      <c r="L44" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="n">
         <v>6</v>
@@ -2786,6 +2914,12 @@
       <c r="P44" t="n">
         <v>10</v>
       </c>
+      <c r="Q44" t="n">
+        <v>3438.374744897959</v>
+      </c>
+      <c r="R44" t="n">
+        <v>3438.374744897959</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2824,13 +2958,9 @@
       <c r="J45" t="n">
         <v>1</v>
       </c>
-      <c r="K45" t="n">
-        <v>2</v>
-      </c>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="n">
-        <v>2</v>
-      </c>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
         <v>6.5</v>
       </c>
@@ -2838,6 +2968,12 @@
         <v>7.5</v>
       </c>
       <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="n">
+        <v>2063.330800937476</v>
+      </c>
+      <c r="R45" t="n">
+        <v>1375.55386729165</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2875,12 +3011,8 @@
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
-      <c r="L46" t="n">
-        <v>2</v>
-      </c>
-      <c r="M46" t="n">
-        <v>2</v>
-      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="n">
         <v>6</v>
       </c>
@@ -2890,6 +3022,12 @@
       <c r="P46" t="n">
         <v>6</v>
       </c>
+      <c r="Q46" t="n">
+        <v>5813.11750968877</v>
+      </c>
+      <c r="R46" t="n">
+        <v>5813.11750968877</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2926,9 +3064,7 @@
         <v>1</v>
       </c>
       <c r="J47" t="inlineStr"/>
-      <c r="K47" t="n">
-        <v>2</v>
-      </c>
+      <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
@@ -2940,6 +3076,12 @@
       <c r="P47" t="n">
         <v>10</v>
       </c>
+      <c r="Q47" t="n">
+        <v>4223.403054818182</v>
+      </c>
+      <c r="R47" t="n">
+        <v>4223.403054818182</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2978,12 +3120,8 @@
       <c r="J48" t="n">
         <v>3</v>
       </c>
-      <c r="K48" t="n">
-        <v>2</v>
-      </c>
-      <c r="L48" t="n">
-        <v>2</v>
-      </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="n">
         <v>6</v>
@@ -2994,6 +3132,12 @@
       <c r="P48" t="n">
         <v>6</v>
       </c>
+      <c r="Q48" t="n">
+        <v>3709.413207049506</v>
+      </c>
+      <c r="R48" t="n">
+        <v>3709.413207049506</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3032,9 +3176,7 @@
       <c r="J49" t="n">
         <v>3</v>
       </c>
-      <c r="K49" t="n">
-        <v>2</v>
-      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="n">
@@ -3046,6 +3188,12 @@
       <c r="P49" t="n">
         <v>6</v>
       </c>
+      <c r="Q49" t="n">
+        <v>4083.582129882433</v>
+      </c>
+      <c r="R49" t="n">
+        <v>4083.582129882433</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3082,12 +3230,8 @@
         <v>2</v>
       </c>
       <c r="J50" t="inlineStr"/>
-      <c r="K50" t="n">
-        <v>2</v>
-      </c>
-      <c r="L50" t="n">
-        <v>2</v>
-      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="n">
         <v>6</v>
@@ -3098,6 +3242,12 @@
       <c r="P50" t="n">
         <v>10</v>
       </c>
+      <c r="Q50" t="n">
+        <v>3316.04685</v>
+      </c>
+      <c r="R50" t="n">
+        <v>3316.04685</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3136,15 +3286,9 @@
       <c r="J51" t="n">
         <v>3</v>
       </c>
-      <c r="K51" t="n">
-        <v>2</v>
-      </c>
-      <c r="L51" t="n">
-        <v>2</v>
-      </c>
-      <c r="M51" t="n">
-        <v>2</v>
-      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
       <c r="N51" t="n">
         <v>6</v>
       </c>
@@ -3154,6 +3298,12 @@
       <c r="P51" t="n">
         <v>6</v>
       </c>
+      <c r="Q51" t="n">
+        <v>2649.114932075875</v>
+      </c>
+      <c r="R51" t="n">
+        <v>2649.114932075875</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3190,13 +3340,9 @@
         <v>1</v>
       </c>
       <c r="J52" t="inlineStr"/>
-      <c r="K52" t="n">
-        <v>2</v>
-      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="n">
-        <v>2</v>
-      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="n">
         <v>5.5</v>
       </c>
@@ -3206,6 +3352,12 @@
       <c r="P52" t="n">
         <v>6</v>
       </c>
+      <c r="Q52" t="n">
+        <v>1396.707552020581</v>
+      </c>
+      <c r="R52" t="n">
+        <v>1396.707552020581</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3247,9 +3399,7 @@
       <c r="K53" t="n">
         <v>2</v>
       </c>
-      <c r="L53" t="n">
-        <v>2</v>
-      </c>
+      <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
         <v>5.5</v>
@@ -3260,6 +3410,12 @@
       <c r="P53" t="n">
         <v>6</v>
       </c>
+      <c r="Q53" t="n">
+        <v>2097.770093457944</v>
+      </c>
+      <c r="R53" t="n">
+        <v>2097.770093457944</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3301,9 +3457,7 @@
       <c r="K54" t="n">
         <v>2</v>
       </c>
-      <c r="L54" t="n">
-        <v>2</v>
-      </c>
+      <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="n">
         <v>5.5</v>
@@ -3314,6 +3468,12 @@
       <c r="P54" t="n">
         <v>6</v>
       </c>
+      <c r="Q54" t="n">
+        <v>2453.640793708587</v>
+      </c>
+      <c r="R54" t="n">
+        <v>2453.640793708587</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3355,12 +3515,8 @@
       <c r="K55" t="n">
         <v>2</v>
       </c>
-      <c r="L55" t="n">
-        <v>2</v>
-      </c>
-      <c r="M55" t="n">
-        <v>2</v>
-      </c>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
         <v>5.5</v>
       </c>
@@ -3370,6 +3526,12 @@
       <c r="P55" t="n">
         <v>8</v>
       </c>
+      <c r="Q55" t="n">
+        <v>2003.49595006928</v>
+      </c>
+      <c r="R55" t="n">
+        <v>2003.49595006928</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3408,13 +3570,11 @@
       <c r="J56" t="n">
         <v>3</v>
       </c>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="n">
-        <v>2</v>
-      </c>
-      <c r="M56" t="n">
-        <v>2</v>
-      </c>
+      <c r="K56" t="n">
+        <v>3</v>
+      </c>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
       <c r="N56" t="n">
         <v>5.5</v>
       </c>
@@ -3424,6 +3584,12 @@
       <c r="P56" t="n">
         <v>8</v>
       </c>
+      <c r="Q56" t="n">
+        <v>976.3144451047938</v>
+      </c>
+      <c r="R56" t="n">
+        <v>976.3144451047938</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3444,7 +3610,7 @@
         <v>21218.6225573449</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -3463,11 +3629,9 @@
         <v>3</v>
       </c>
       <c r="K57" t="inlineStr"/>
-      <c r="L57" t="n">
-        <v>2</v>
-      </c>
+      <c r="L57" t="inlineStr"/>
       <c r="M57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N57" t="n">
         <v>5.5</v>
@@ -3478,6 +3642,12 @@
       <c r="P57" t="n">
         <v>8</v>
       </c>
+      <c r="Q57" t="n">
+        <v>628.9810203563475</v>
+      </c>
+      <c r="R57" t="n">
+        <v>471.7357652672606</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3519,12 +3689,8 @@
       <c r="K58" t="n">
         <v>2</v>
       </c>
-      <c r="L58" t="n">
-        <v>2</v>
-      </c>
-      <c r="M58" t="n">
-        <v>2</v>
-      </c>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
       <c r="N58" t="n">
         <v>5.5</v>
       </c>
@@ -3534,6 +3700,12 @@
       <c r="P58" t="n">
         <v>6</v>
       </c>
+      <c r="Q58" t="n">
+        <v>1940.702872862183</v>
+      </c>
+      <c r="R58" t="n">
+        <v>1940.702872862183</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3575,9 +3747,7 @@
       <c r="K59" t="n">
         <v>2</v>
       </c>
-      <c r="L59" t="n">
-        <v>2</v>
-      </c>
+      <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="n">
         <v>5.5</v>
@@ -3588,6 +3758,12 @@
       <c r="P59" t="n">
         <v>6</v>
       </c>
+      <c r="Q59" t="n">
+        <v>1097.979282918159</v>
+      </c>
+      <c r="R59" t="n">
+        <v>1097.979282918159</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3623,14 +3799,10 @@
         <v>3</v>
       </c>
       <c r="K60" t="n">
-        <v>1</v>
-      </c>
-      <c r="L60" t="n">
-        <v>2</v>
-      </c>
-      <c r="M60" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
       <c r="N60" t="n">
         <v>6</v>
       </c>
@@ -3640,6 +3812,8 @@
       <c r="P60" t="n">
         <v>8</v>
       </c>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3675,12 +3849,10 @@
         <v>3</v>
       </c>
       <c r="K61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L61" t="inlineStr"/>
-      <c r="M61" t="n">
-        <v>2</v>
-      </c>
+      <c r="M61" t="inlineStr"/>
       <c r="N61" t="n">
         <v>6</v>
       </c>
@@ -3690,6 +3862,8 @@
       <c r="P61" t="n">
         <v>8</v>
       </c>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3738,6 +3912,12 @@
       <c r="P62" t="n">
         <v>12</v>
       </c>
+      <c r="Q62" t="n">
+        <v>1863.035368009254</v>
+      </c>
+      <c r="R62" t="n">
+        <v>1863.035368009254</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3777,14 +3957,10 @@
         <v>3</v>
       </c>
       <c r="K63" t="n">
-        <v>1</v>
-      </c>
-      <c r="L63" t="n">
-        <v>2</v>
-      </c>
-      <c r="M63" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
       <c r="N63" t="n">
         <v>5.5</v>
       </c>
@@ -3794,6 +3970,12 @@
       <c r="P63" t="n">
         <v>6</v>
       </c>
+      <c r="Q63" t="n">
+        <v>1674.079528746844</v>
+      </c>
+      <c r="R63" t="n">
+        <v>1255.559646560133</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3814,7 +3996,7 @@
         <v>10048</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3833,9 +4015,7 @@
         <v>3</v>
       </c>
       <c r="K64" t="inlineStr"/>
-      <c r="L64" t="n">
-        <v>1</v>
-      </c>
+      <c r="L64" t="inlineStr"/>
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="n">
         <v>6</v>
@@ -3845,6 +4025,12 @@
       </c>
       <c r="P64" t="n">
         <v>8</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>1720.864367816092</v>
+      </c>
+      <c r="R64" t="n">
+        <v>1290.648275862069</v>
       </c>
     </row>
     <row r="65">
@@ -3881,11 +4067,9 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="n">
-        <v>2</v>
-      </c>
-      <c r="L65" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L65" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="n">
         <v>6</v>
@@ -3896,6 +4080,12 @@
       <c r="P65" t="n">
         <v>10</v>
       </c>
+      <c r="Q65" t="n">
+        <v>4145.53255319149</v>
+      </c>
+      <c r="R65" t="n">
+        <v>4145.53255319149</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3934,13 +4124,9 @@
       <c r="J66" t="n">
         <v>1</v>
       </c>
-      <c r="K66" t="n">
-        <v>2</v>
-      </c>
+      <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="n">
-        <v>2</v>
-      </c>
+      <c r="M66" t="inlineStr"/>
       <c r="N66" t="n">
         <v>6.5</v>
       </c>
@@ -3948,6 +4134,12 @@
         <v>7.5</v>
       </c>
       <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="n">
+        <v>2150.111153846154</v>
+      </c>
+      <c r="R66" t="n">
+        <v>1433.407435897436</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3985,12 +4177,8 @@
       </c>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
-      <c r="L67" t="n">
-        <v>2</v>
-      </c>
-      <c r="M67" t="n">
-        <v>2</v>
-      </c>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
       <c r="N67" t="n">
         <v>6</v>
       </c>
@@ -4000,6 +4188,12 @@
       <c r="P67" t="n">
         <v>6</v>
       </c>
+      <c r="Q67" t="n">
+        <v>7413.207647058823</v>
+      </c>
+      <c r="R67" t="n">
+        <v>7413.207647058823</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4036,9 +4230,7 @@
         <v>1</v>
       </c>
       <c r="J68" t="inlineStr"/>
-      <c r="K68" t="n">
-        <v>2</v>
-      </c>
+      <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
       <c r="M68" t="inlineStr"/>
       <c r="N68" t="n">
@@ -4050,6 +4242,12 @@
       <c r="P68" t="n">
         <v>10</v>
       </c>
+      <c r="Q68" t="n">
+        <v>3123.984482758621</v>
+      </c>
+      <c r="R68" t="n">
+        <v>3123.984482758621</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4088,12 +4286,8 @@
       <c r="J69" t="n">
         <v>3</v>
       </c>
-      <c r="K69" t="n">
-        <v>2</v>
-      </c>
-      <c r="L69" t="n">
-        <v>2</v>
-      </c>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="n">
         <v>6</v>
@@ -4104,6 +4298,12 @@
       <c r="P69" t="n">
         <v>6</v>
       </c>
+      <c r="Q69" t="n">
+        <v>3210.606386554622</v>
+      </c>
+      <c r="R69" t="n">
+        <v>3210.606386554622</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4142,9 +4342,7 @@
       <c r="J70" t="n">
         <v>3</v>
       </c>
-      <c r="K70" t="n">
-        <v>2</v>
-      </c>
+      <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="n">
@@ -4156,6 +4354,12 @@
       <c r="P70" t="n">
         <v>6</v>
       </c>
+      <c r="Q70" t="n">
+        <v>3628.137352941176</v>
+      </c>
+      <c r="R70" t="n">
+        <v>3628.137352941176</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4192,12 +4396,8 @@
         <v>2</v>
       </c>
       <c r="J71" t="inlineStr"/>
-      <c r="K71" t="n">
-        <v>2</v>
-      </c>
-      <c r="L71" t="n">
-        <v>2</v>
-      </c>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="n">
         <v>6</v>
@@ -4208,6 +4408,12 @@
       <c r="P71" t="n">
         <v>10</v>
       </c>
+      <c r="Q71" t="n">
+        <v>3726.6645</v>
+      </c>
+      <c r="R71" t="n">
+        <v>3726.6645</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4246,15 +4452,9 @@
       <c r="J72" t="n">
         <v>3</v>
       </c>
-      <c r="K72" t="n">
-        <v>2</v>
-      </c>
-      <c r="L72" t="n">
-        <v>2</v>
-      </c>
-      <c r="M72" t="n">
-        <v>2</v>
-      </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
       <c r="N72" t="n">
         <v>6</v>
       </c>
@@ -4264,6 +4464,12 @@
       <c r="P72" t="n">
         <v>6</v>
       </c>
+      <c r="Q72" t="n">
+        <v>3005.462077922078</v>
+      </c>
+      <c r="R72" t="n">
+        <v>3005.462077922078</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4300,13 +4506,9 @@
         <v>1</v>
       </c>
       <c r="J73" t="inlineStr"/>
-      <c r="K73" t="n">
-        <v>2</v>
-      </c>
+      <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
-      <c r="M73" t="n">
-        <v>2</v>
-      </c>
+      <c r="M73" t="inlineStr"/>
       <c r="N73" t="n">
         <v>5.5</v>
       </c>
@@ -4316,6 +4518,12 @@
       <c r="P73" t="n">
         <v>6</v>
       </c>
+      <c r="Q73" t="n">
+        <v>1840.81442384106</v>
+      </c>
+      <c r="R73" t="n">
+        <v>1840.81442384106</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4357,9 +4565,7 @@
       <c r="K74" t="n">
         <v>2</v>
       </c>
-      <c r="L74" t="n">
-        <v>2</v>
-      </c>
+      <c r="L74" t="inlineStr"/>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="n">
         <v>5.5</v>
@@ -4370,6 +4576,12 @@
       <c r="P74" t="n">
         <v>6</v>
       </c>
+      <c r="Q74" t="n">
+        <v>2114.835185185185</v>
+      </c>
+      <c r="R74" t="n">
+        <v>2114.835185185185</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4411,9 +4623,7 @@
       <c r="K75" t="n">
         <v>2</v>
       </c>
-      <c r="L75" t="n">
-        <v>2</v>
-      </c>
+      <c r="L75" t="inlineStr"/>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="n">
         <v>5.5</v>
@@ -4424,6 +4634,12 @@
       <c r="P75" t="n">
         <v>6</v>
       </c>
+      <c r="Q75" t="n">
+        <v>2416.81875</v>
+      </c>
+      <c r="R75" t="n">
+        <v>2416.81875</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4465,12 +4681,8 @@
       <c r="K76" t="n">
         <v>2</v>
       </c>
-      <c r="L76" t="n">
-        <v>2</v>
-      </c>
-      <c r="M76" t="n">
-        <v>2</v>
-      </c>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
       <c r="N76" t="n">
         <v>5.5</v>
       </c>
@@ -4480,6 +4692,12 @@
       <c r="P76" t="n">
         <v>8</v>
       </c>
+      <c r="Q76" t="n">
+        <v>1936.964615384615</v>
+      </c>
+      <c r="R76" t="n">
+        <v>1936.964615384615</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4518,13 +4736,11 @@
       <c r="J77" t="n">
         <v>3</v>
       </c>
-      <c r="K77" t="inlineStr"/>
-      <c r="L77" t="n">
-        <v>2</v>
-      </c>
-      <c r="M77" t="n">
-        <v>2</v>
-      </c>
+      <c r="K77" t="n">
+        <v>3</v>
+      </c>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
       <c r="N77" t="n">
         <v>5.5</v>
       </c>
@@ -4534,6 +4750,12 @@
       <c r="P77" t="n">
         <v>8</v>
       </c>
+      <c r="Q77" t="n">
+        <v>1184.96296875</v>
+      </c>
+      <c r="R77" t="n">
+        <v>1184.96296875</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4554,7 +4776,7 @@
         <v>23892</v>
       </c>
       <c r="F78" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -4573,11 +4795,9 @@
         <v>3</v>
       </c>
       <c r="K78" t="inlineStr"/>
-      <c r="L78" t="n">
-        <v>2</v>
-      </c>
+      <c r="L78" t="inlineStr"/>
       <c r="M78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N78" t="n">
         <v>5.5</v>
@@ -4588,6 +4808,12 @@
       <c r="P78" t="n">
         <v>8</v>
       </c>
+      <c r="Q78" t="n">
+        <v>674.3886041189932</v>
+      </c>
+      <c r="R78" t="n">
+        <v>505.7914530892449</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4629,12 +4855,8 @@
       <c r="K79" t="n">
         <v>2</v>
       </c>
-      <c r="L79" t="n">
-        <v>2</v>
-      </c>
-      <c r="M79" t="n">
-        <v>2</v>
-      </c>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
       <c r="N79" t="n">
         <v>5.5</v>
       </c>
@@ -4644,6 +4866,12 @@
       <c r="P79" t="n">
         <v>6</v>
       </c>
+      <c r="Q79" t="n">
+        <v>1906.265882352941</v>
+      </c>
+      <c r="R79" t="n">
+        <v>1906.265882352941</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4685,9 +4913,7 @@
       <c r="K80" t="n">
         <v>2</v>
       </c>
-      <c r="L80" t="n">
-        <v>2</v>
-      </c>
+      <c r="L80" t="inlineStr"/>
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="n">
         <v>5.5</v>
@@ -4698,6 +4924,12 @@
       <c r="P80" t="n">
         <v>6</v>
       </c>
+      <c r="Q80" t="n">
+        <v>1036.7445</v>
+      </c>
+      <c r="R80" t="n">
+        <v>1036.7445</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4735,14 +4967,10 @@
         <v>3</v>
       </c>
       <c r="K81" t="n">
-        <v>1</v>
-      </c>
-      <c r="L81" t="n">
-        <v>2</v>
-      </c>
-      <c r="M81" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
       <c r="N81" t="n">
         <v>6</v>
       </c>
@@ -4752,6 +4980,12 @@
       <c r="P81" t="n">
         <v>8</v>
       </c>
+      <c r="Q81" t="n">
+        <v>9248.006352357321</v>
+      </c>
+      <c r="R81" t="n">
+        <v>6936.004764267991</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4789,12 +5023,10 @@
         <v>3</v>
       </c>
       <c r="K82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L82" t="inlineStr"/>
-      <c r="M82" t="n">
-        <v>2</v>
-      </c>
+      <c r="M82" t="inlineStr"/>
       <c r="N82" t="n">
         <v>6</v>
       </c>
@@ -4803,6 +5035,12 @@
       </c>
       <c r="P82" t="n">
         <v>8</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>9248.006352357321</v>
+      </c>
+      <c r="R82" t="n">
+        <v>6936.004764267991</v>
       </c>
     </row>
     <row r="83">
@@ -4852,6 +5090,12 @@
       <c r="P83" t="n">
         <v>12</v>
       </c>
+      <c r="Q83" t="n">
+        <v>1845.888</v>
+      </c>
+      <c r="R83" t="n">
+        <v>1845.888</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4891,14 +5135,10 @@
         <v>3</v>
       </c>
       <c r="K84" t="n">
-        <v>1</v>
-      </c>
-      <c r="L84" t="n">
-        <v>2</v>
-      </c>
-      <c r="M84" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
       <c r="N84" t="n">
         <v>5.5</v>
       </c>
@@ -4908,6 +5148,12 @@
       <c r="P84" t="n">
         <v>6</v>
       </c>
+      <c r="Q84" t="n">
+        <v>2333.010835266821</v>
+      </c>
+      <c r="R84" t="n">
+        <v>1749.758126450116</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4928,7 +5174,7 @@
         <v>8860</v>
       </c>
       <c r="F85" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -4947,9 +5193,7 @@
         <v>3</v>
       </c>
       <c r="K85" t="inlineStr"/>
-      <c r="L85" t="n">
-        <v>1</v>
-      </c>
+      <c r="L85" t="inlineStr"/>
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="n">
         <v>6</v>
@@ -4959,6 +5203,12 @@
       </c>
       <c r="P85" t="n">
         <v>8</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>1909.187096774194</v>
+      </c>
+      <c r="R85" t="n">
+        <v>1431.890322580645</v>
       </c>
     </row>
     <row r="86">
@@ -4995,11 +5245,9 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="n">
-        <v>2</v>
-      </c>
-      <c r="L86" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L86" t="inlineStr"/>
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="n">
         <v>6</v>
@@ -5010,6 +5258,12 @@
       <c r="P86" t="n">
         <v>10</v>
       </c>
+      <c r="Q86" t="n">
+        <v>5761.247346938775</v>
+      </c>
+      <c r="R86" t="n">
+        <v>5761.247346938775</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5048,13 +5302,9 @@
       <c r="J87" t="n">
         <v>1</v>
       </c>
-      <c r="K87" t="n">
-        <v>2</v>
-      </c>
+      <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
-      <c r="M87" t="n">
-        <v>2</v>
-      </c>
+      <c r="M87" t="inlineStr"/>
       <c r="N87" t="n">
         <v>6.5</v>
       </c>
@@ -5062,6 +5312,12 @@
         <v>7.5</v>
       </c>
       <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="n">
+        <v>2518.16858490566</v>
+      </c>
+      <c r="R87" t="n">
+        <v>1678.779056603773</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5099,12 +5355,8 @@
       </c>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
-      <c r="L88" t="n">
-        <v>2</v>
-      </c>
-      <c r="M88" t="n">
-        <v>2</v>
-      </c>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
       <c r="N88" t="n">
         <v>6</v>
       </c>
@@ -5114,6 +5366,12 @@
       <c r="P88" t="n">
         <v>6</v>
       </c>
+      <c r="Q88" t="n">
+        <v>10521.04283054003</v>
+      </c>
+      <c r="R88" t="n">
+        <v>10521.04283054003</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5150,9 +5408,7 @@
         <v>1</v>
       </c>
       <c r="J89" t="inlineStr"/>
-      <c r="K89" t="n">
-        <v>2</v>
-      </c>
+      <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="n">
@@ -5164,6 +5420,12 @@
       <c r="P89" t="n">
         <v>10</v>
       </c>
+      <c r="Q89" t="n">
+        <v>3446.729452054795</v>
+      </c>
+      <c r="R89" t="n">
+        <v>3446.729452054795</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5202,12 +5464,8 @@
       <c r="J90" t="n">
         <v>3</v>
       </c>
-      <c r="K90" t="n">
-        <v>2</v>
-      </c>
-      <c r="L90" t="n">
-        <v>2</v>
-      </c>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="n">
         <v>6</v>
@@ -5218,6 +5476,12 @@
       <c r="P90" t="n">
         <v>6</v>
       </c>
+      <c r="Q90" t="n">
+        <v>4838.570249147751</v>
+      </c>
+      <c r="R90" t="n">
+        <v>4838.570249147751</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5256,9 +5520,7 @@
       <c r="J91" t="n">
         <v>3</v>
       </c>
-      <c r="K91" t="n">
-        <v>2</v>
-      </c>
+      <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="n">
@@ -5270,6 +5532,12 @@
       <c r="P91" t="n">
         <v>6</v>
       </c>
+      <c r="Q91" t="n">
+        <v>3644.017777777778</v>
+      </c>
+      <c r="R91" t="n">
+        <v>3644.017777777778</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5306,12 +5574,8 @@
         <v>2</v>
       </c>
       <c r="J92" t="inlineStr"/>
-      <c r="K92" t="n">
-        <v>2</v>
-      </c>
-      <c r="L92" t="n">
-        <v>2</v>
-      </c>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="n">
         <v>6</v>
@@ -5322,6 +5586,12 @@
       <c r="P92" t="n">
         <v>10</v>
       </c>
+      <c r="Q92" t="n">
+        <v>4347.21</v>
+      </c>
+      <c r="R92" t="n">
+        <v>4347.21</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5360,15 +5630,9 @@
       <c r="J93" t="n">
         <v>3</v>
       </c>
-      <c r="K93" t="n">
-        <v>2</v>
-      </c>
-      <c r="L93" t="n">
-        <v>2</v>
-      </c>
-      <c r="M93" t="n">
-        <v>2</v>
-      </c>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
       <c r="N93" t="n">
         <v>6</v>
       </c>
@@ -5378,6 +5642,12 @@
       <c r="P93" t="n">
         <v>6</v>
       </c>
+      <c r="Q93" t="n">
+        <v>3263.345492443981</v>
+      </c>
+      <c r="R93" t="n">
+        <v>3263.345492443981</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5414,13 +5684,9 @@
         <v>1</v>
       </c>
       <c r="J94" t="inlineStr"/>
-      <c r="K94" t="n">
-        <v>2</v>
-      </c>
+      <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
-      <c r="M94" t="n">
-        <v>2</v>
-      </c>
+      <c r="M94" t="inlineStr"/>
       <c r="N94" t="n">
         <v>5.5</v>
       </c>
@@ -5430,6 +5696,12 @@
       <c r="P94" t="n">
         <v>6</v>
       </c>
+      <c r="Q94" t="n">
+        <v>3287.093875</v>
+      </c>
+      <c r="R94" t="n">
+        <v>3287.093875</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5471,9 +5743,7 @@
       <c r="K95" t="n">
         <v>2</v>
       </c>
-      <c r="L95" t="n">
-        <v>2</v>
-      </c>
+      <c r="L95" t="inlineStr"/>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="n">
         <v>5.5</v>
@@ -5484,6 +5754,12 @@
       <c r="P95" t="n">
         <v>6</v>
       </c>
+      <c r="Q95" t="n">
+        <v>2247.4875</v>
+      </c>
+      <c r="R95" t="n">
+        <v>2247.4875</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5525,9 +5801,7 @@
       <c r="K96" t="n">
         <v>2</v>
       </c>
-      <c r="L96" t="n">
-        <v>2</v>
-      </c>
+      <c r="L96" t="inlineStr"/>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="n">
         <v>5.5</v>
@@ -5538,6 +5812,12 @@
       <c r="P96" t="n">
         <v>6</v>
       </c>
+      <c r="Q96" t="n">
+        <v>2372.954838709677</v>
+      </c>
+      <c r="R96" t="n">
+        <v>2372.954838709677</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5579,12 +5859,8 @@
       <c r="K97" t="n">
         <v>2</v>
       </c>
-      <c r="L97" t="n">
-        <v>2</v>
-      </c>
-      <c r="M97" t="n">
-        <v>2</v>
-      </c>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
       <c r="N97" t="n">
         <v>5.5</v>
       </c>
@@ -5594,6 +5870,12 @@
       <c r="P97" t="n">
         <v>8</v>
       </c>
+      <c r="Q97" t="n">
+        <v>2583.9</v>
+      </c>
+      <c r="R97" t="n">
+        <v>2583.9</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5632,13 +5914,11 @@
       <c r="J98" t="n">
         <v>3</v>
       </c>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="n">
-        <v>2</v>
-      </c>
-      <c r="M98" t="n">
-        <v>2</v>
-      </c>
+      <c r="K98" t="n">
+        <v>3</v>
+      </c>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
       <c r="N98" t="n">
         <v>5.5</v>
       </c>
@@ -5648,6 +5928,12 @@
       <c r="P98" t="n">
         <v>8</v>
       </c>
+      <c r="Q98" t="n">
+        <v>1123.05815056415</v>
+      </c>
+      <c r="R98" t="n">
+        <v>1123.05815056415</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5668,7 +5954,7 @@
         <v>26471</v>
       </c>
       <c r="F99" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -5687,11 +5973,9 @@
         <v>3</v>
       </c>
       <c r="K99" t="inlineStr"/>
-      <c r="L99" t="n">
-        <v>2</v>
-      </c>
+      <c r="L99" t="inlineStr"/>
       <c r="M99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N99" t="n">
         <v>5.5</v>
@@ -5702,6 +5986,12 @@
       <c r="P99" t="n">
         <v>8</v>
       </c>
+      <c r="Q99" t="n">
+        <v>983.5940090600227</v>
+      </c>
+      <c r="R99" t="n">
+        <v>737.6955067950171</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5743,12 +6033,8 @@
       <c r="K100" t="n">
         <v>2</v>
       </c>
-      <c r="L100" t="n">
-        <v>2</v>
-      </c>
-      <c r="M100" t="n">
-        <v>2</v>
-      </c>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
       <c r="N100" t="n">
         <v>5.5</v>
       </c>
@@ -5758,6 +6044,12 @@
       <c r="P100" t="n">
         <v>6</v>
       </c>
+      <c r="Q100" t="n">
+        <v>1686.959555312092</v>
+      </c>
+      <c r="R100" t="n">
+        <v>1686.959555312092</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5799,9 +6091,7 @@
       <c r="K101" t="n">
         <v>2</v>
       </c>
-      <c r="L101" t="n">
-        <v>2</v>
-      </c>
+      <c r="L101" t="inlineStr"/>
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="n">
         <v>5.5</v>
@@ -5812,6 +6102,12 @@
       <c r="P101" t="n">
         <v>6</v>
       </c>
+      <c r="Q101" t="n">
+        <v>1260.862104970884</v>
+      </c>
+      <c r="R101" t="n">
+        <v>1260.862104970884</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5849,14 +6145,10 @@
         <v>3</v>
       </c>
       <c r="K102" t="n">
-        <v>1</v>
-      </c>
-      <c r="L102" t="n">
-        <v>2</v>
-      </c>
-      <c r="M102" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
       <c r="N102" t="n">
         <v>6</v>
       </c>
@@ -5866,6 +6158,12 @@
       <c r="P102" t="n">
         <v>8</v>
       </c>
+      <c r="Q102" t="n">
+        <v>10124.40475404457</v>
+      </c>
+      <c r="R102" t="n">
+        <v>7593.303565533428</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5903,12 +6201,10 @@
         <v>3</v>
       </c>
       <c r="K103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L103" t="inlineStr"/>
-      <c r="M103" t="n">
-        <v>2</v>
-      </c>
+      <c r="M103" t="inlineStr"/>
       <c r="N103" t="n">
         <v>6</v>
       </c>
@@ -5917,6 +6213,12 @@
       </c>
       <c r="P103" t="n">
         <v>8</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>10124.40475404457</v>
+      </c>
+      <c r="R103" t="n">
+        <v>7593.303565533428</v>
       </c>
     </row>
     <row r="104">
@@ -5966,6 +6268,12 @@
       <c r="P104" t="n">
         <v>12</v>
       </c>
+      <c r="Q104" t="n">
+        <v>2515.80531910795</v>
+      </c>
+      <c r="R104" t="n">
+        <v>2515.80531910795</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6005,14 +6313,10 @@
         <v>3</v>
       </c>
       <c r="K105" t="n">
-        <v>1</v>
-      </c>
-      <c r="L105" t="n">
-        <v>2</v>
-      </c>
-      <c r="M105" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
       <c r="N105" t="n">
         <v>5.5</v>
       </c>
@@ -6022,6 +6326,12 @@
       <c r="P105" t="n">
         <v>6</v>
       </c>
+      <c r="Q105" t="n">
+        <v>2722.604930875576</v>
+      </c>
+      <c r="R105" t="n">
+        <v>2041.953698156682</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -6042,7 +6352,7 @@
         <v>8920</v>
       </c>
       <c r="F106" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -6061,9 +6371,7 @@
         <v>3</v>
       </c>
       <c r="K106" t="inlineStr"/>
-      <c r="L106" t="n">
-        <v>1</v>
-      </c>
+      <c r="L106" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="n">
         <v>6</v>
@@ -6073,6 +6381,12 @@
       </c>
       <c r="P106" t="n">
         <v>8</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>2301.935483870968</v>
+      </c>
+      <c r="R106" t="n">
+        <v>1726.451612903226</v>
       </c>
     </row>
     <row r="107">
@@ -6109,11 +6423,9 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="n">
-        <v>2</v>
-      </c>
-      <c r="L107" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L107" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="n">
         <v>6</v>
@@ -6124,6 +6436,12 @@
       <c r="P107" t="n">
         <v>10</v>
       </c>
+      <c r="Q107" t="n">
+        <v>6378.861176470588</v>
+      </c>
+      <c r="R107" t="n">
+        <v>6378.861176470588</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -6162,13 +6480,9 @@
       <c r="J108" t="n">
         <v>1</v>
       </c>
-      <c r="K108" t="n">
-        <v>2</v>
-      </c>
+      <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
-      <c r="M108" t="n">
-        <v>2</v>
-      </c>
+      <c r="M108" t="inlineStr"/>
       <c r="N108" t="n">
         <v>6.5</v>
       </c>
@@ -6176,6 +6490,12 @@
         <v>7.5</v>
       </c>
       <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="n">
+        <v>3524.243584905661</v>
+      </c>
+      <c r="R108" t="n">
+        <v>2349.49572327044</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -6213,12 +6533,8 @@
       </c>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
-      <c r="L109" t="n">
-        <v>2</v>
-      </c>
-      <c r="M109" t="n">
-        <v>2</v>
-      </c>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
       <c r="N109" t="n">
         <v>6</v>
       </c>
@@ -6228,6 +6544,12 @@
       <c r="P109" t="n">
         <v>6</v>
       </c>
+      <c r="Q109" t="n">
+        <v>11776.28</v>
+      </c>
+      <c r="R109" t="n">
+        <v>11776.28</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -6264,9 +6586,7 @@
         <v>1</v>
       </c>
       <c r="J110" t="inlineStr"/>
-      <c r="K110" t="n">
-        <v>2</v>
-      </c>
+      <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="n">
@@ -6278,6 +6598,12 @@
       <c r="P110" t="n">
         <v>10</v>
       </c>
+      <c r="Q110" t="n">
+        <v>3762.933103448276</v>
+      </c>
+      <c r="R110" t="n">
+        <v>3762.933103448276</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -6316,12 +6642,8 @@
       <c r="J111" t="n">
         <v>3</v>
       </c>
-      <c r="K111" t="n">
-        <v>2</v>
-      </c>
-      <c r="L111" t="n">
-        <v>2</v>
-      </c>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
       <c r="N111" t="n">
         <v>6</v>
@@ -6332,6 +6654,12 @@
       <c r="P111" t="n">
         <v>6</v>
       </c>
+      <c r="Q111" t="n">
+        <v>5065.47868852459</v>
+      </c>
+      <c r="R111" t="n">
+        <v>5065.47868852459</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -6370,9 +6698,7 @@
       <c r="J112" t="n">
         <v>3</v>
       </c>
-      <c r="K112" t="n">
-        <v>2</v>
-      </c>
+      <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="n">
@@ -6384,6 +6710,12 @@
       <c r="P112" t="n">
         <v>6</v>
       </c>
+      <c r="Q112" t="n">
+        <v>3686.126691176471</v>
+      </c>
+      <c r="R112" t="n">
+        <v>3686.126691176471</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6420,12 +6752,8 @@
         <v>2</v>
       </c>
       <c r="J113" t="inlineStr"/>
-      <c r="K113" t="n">
-        <v>2</v>
-      </c>
-      <c r="L113" t="n">
-        <v>2</v>
-      </c>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="n">
         <v>6</v>
@@ -6436,6 +6764,12 @@
       <c r="P113" t="n">
         <v>10</v>
       </c>
+      <c r="Q113" t="n">
+        <v>4359.978333333333</v>
+      </c>
+      <c r="R113" t="n">
+        <v>4359.978333333333</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6474,15 +6808,9 @@
       <c r="J114" t="n">
         <v>3</v>
       </c>
-      <c r="K114" t="n">
-        <v>2</v>
-      </c>
-      <c r="L114" t="n">
-        <v>2</v>
-      </c>
-      <c r="M114" t="n">
-        <v>2</v>
-      </c>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
       <c r="N114" t="n">
         <v>6</v>
       </c>
@@ -6492,6 +6820,12 @@
       <c r="P114" t="n">
         <v>6</v>
       </c>
+      <c r="Q114" t="n">
+        <v>3947.360375</v>
+      </c>
+      <c r="R114" t="n">
+        <v>3947.360375</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6528,13 +6862,9 @@
         <v>1</v>
       </c>
       <c r="J115" t="inlineStr"/>
-      <c r="K115" t="n">
-        <v>2</v>
-      </c>
+      <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
-      <c r="M115" t="n">
-        <v>2</v>
-      </c>
+      <c r="M115" t="inlineStr"/>
       <c r="N115" t="n">
         <v>5.5</v>
       </c>
@@ -6544,6 +6874,12 @@
       <c r="P115" t="n">
         <v>6</v>
       </c>
+      <c r="Q115" t="n">
+        <v>3346.066705882353</v>
+      </c>
+      <c r="R115" t="n">
+        <v>3346.066705882353</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6585,9 +6921,7 @@
       <c r="K116" t="n">
         <v>2</v>
       </c>
-      <c r="L116" t="n">
-        <v>2</v>
-      </c>
+      <c r="L116" t="inlineStr"/>
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="n">
         <v>5.5</v>
@@ -6598,6 +6932,12 @@
       <c r="P116" t="n">
         <v>6</v>
       </c>
+      <c r="Q116" t="n">
+        <v>2021.627586206897</v>
+      </c>
+      <c r="R116" t="n">
+        <v>2021.627586206897</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6639,9 +6979,7 @@
       <c r="K117" t="n">
         <v>2</v>
       </c>
-      <c r="L117" t="n">
-        <v>2</v>
-      </c>
+      <c r="L117" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="n">
         <v>5.5</v>
@@ -6652,6 +6990,12 @@
       <c r="P117" t="n">
         <v>6</v>
       </c>
+      <c r="Q117" t="n">
+        <v>2155.034482758621</v>
+      </c>
+      <c r="R117" t="n">
+        <v>2155.034482758621</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6693,12 +7037,8 @@
       <c r="K118" t="n">
         <v>2</v>
       </c>
-      <c r="L118" t="n">
-        <v>2</v>
-      </c>
-      <c r="M118" t="n">
-        <v>2</v>
-      </c>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
       <c r="N118" t="n">
         <v>5.5</v>
       </c>
@@ -6708,6 +7048,12 @@
       <c r="P118" t="n">
         <v>8</v>
       </c>
+      <c r="Q118" t="n">
+        <v>3163.977804878049</v>
+      </c>
+      <c r="R118" t="n">
+        <v>3163.977804878049</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6746,13 +7092,11 @@
       <c r="J119" t="n">
         <v>3</v>
       </c>
-      <c r="K119" t="inlineStr"/>
-      <c r="L119" t="n">
-        <v>2</v>
-      </c>
-      <c r="M119" t="n">
-        <v>2</v>
-      </c>
+      <c r="K119" t="n">
+        <v>3</v>
+      </c>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
       <c r="N119" t="n">
         <v>5.5</v>
       </c>
@@ -6762,6 +7106,12 @@
       <c r="P119" t="n">
         <v>8</v>
       </c>
+      <c r="Q119" t="n">
+        <v>1876.37890625</v>
+      </c>
+      <c r="R119" t="n">
+        <v>1876.37890625</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6782,7 +7132,7 @@
         <v>25688</v>
       </c>
       <c r="F120" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -6801,11 +7151,9 @@
         <v>3</v>
       </c>
       <c r="K120" t="inlineStr"/>
-      <c r="L120" t="n">
-        <v>2</v>
-      </c>
+      <c r="L120" t="inlineStr"/>
       <c r="M120" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N120" t="n">
         <v>5.5</v>
@@ -6816,6 +7164,12 @@
       <c r="P120" t="n">
         <v>8</v>
       </c>
+      <c r="Q120" t="n">
+        <v>1325.91595959596</v>
+      </c>
+      <c r="R120" t="n">
+        <v>994.4369696969698</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6857,12 +7211,8 @@
       <c r="K121" t="n">
         <v>2</v>
       </c>
-      <c r="L121" t="n">
-        <v>2</v>
-      </c>
-      <c r="M121" t="n">
-        <v>2</v>
-      </c>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
       <c r="N121" t="n">
         <v>5.5</v>
       </c>
@@ -6872,6 +7222,12 @@
       <c r="P121" t="n">
         <v>6</v>
       </c>
+      <c r="Q121" t="n">
+        <v>1660.211153846154</v>
+      </c>
+      <c r="R121" t="n">
+        <v>1660.211153846154</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6913,9 +7269,7 @@
       <c r="K122" t="n">
         <v>2</v>
       </c>
-      <c r="L122" t="n">
-        <v>2</v>
-      </c>
+      <c r="L122" t="inlineStr"/>
       <c r="M122" t="inlineStr"/>
       <c r="N122" t="n">
         <v>5.5</v>
@@ -6926,6 +7280,12 @@
       <c r="P122" t="n">
         <v>6</v>
       </c>
+      <c r="Q122" t="n">
+        <v>1738.342177419355</v>
+      </c>
+      <c r="R122" t="n">
+        <v>1738.342177419355</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -6963,14 +7323,10 @@
         <v>3</v>
       </c>
       <c r="K123" t="n">
-        <v>1</v>
-      </c>
-      <c r="L123" t="n">
-        <v>2</v>
-      </c>
-      <c r="M123" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
       <c r="N123" t="n">
         <v>6</v>
       </c>
@@ -6980,6 +7336,12 @@
       <c r="P123" t="n">
         <v>8</v>
       </c>
+      <c r="Q123" t="n">
+        <v>9168.789552631579</v>
+      </c>
+      <c r="R123" t="n">
+        <v>6876.592164473685</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -7017,12 +7379,10 @@
         <v>3</v>
       </c>
       <c r="K124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L124" t="inlineStr"/>
-      <c r="M124" t="n">
-        <v>2</v>
-      </c>
+      <c r="M124" t="inlineStr"/>
       <c r="N124" t="n">
         <v>6</v>
       </c>
@@ -7031,6 +7391,12 @@
       </c>
       <c r="P124" t="n">
         <v>8</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>9168.789552631579</v>
+      </c>
+      <c r="R124" t="n">
+        <v>6876.592164473685</v>
       </c>
     </row>
     <row r="125">
@@ -7080,6 +7446,12 @@
       <c r="P125" t="n">
         <v>12</v>
       </c>
+      <c r="Q125" t="n">
+        <v>2360.575</v>
+      </c>
+      <c r="R125" t="n">
+        <v>2360.575</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -7119,14 +7491,10 @@
         <v>3</v>
       </c>
       <c r="K126" t="n">
-        <v>1</v>
-      </c>
-      <c r="L126" t="n">
-        <v>2</v>
-      </c>
-      <c r="M126" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
       <c r="N126" t="n">
         <v>5.5</v>
       </c>
@@ -7135,6 +7503,12 @@
       </c>
       <c r="P126" t="n">
         <v>6</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>2227.487514285714</v>
+      </c>
+      <c r="R126" t="n">
+        <v>1670.615635714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>